<commit_message>
add dijkstra_new() which tracks the path
</commit_message>
<xml_diff>
--- a/Proj1.xlsx
+++ b/Proj1.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanch/Dropbox/f2017/cis677/Proj1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20380" yWindow="460" windowWidth="17700" windowHeight="18860" tabRatio="500"/>
+    <workbookView xWindow="-20385" yWindow="465" windowWidth="17700" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="24">
   <si>
     <t>S1</t>
   </si>
@@ -82,12 +74,30 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +117,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,6 +352,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -427,7 +447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -604,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,24 +632,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="1" customWidth="1"/>
-    <col min="2" max="7" width="5.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16" width="5.83203125" style="3" customWidth="1"/>
-    <col min="17" max="26" width="5.83203125" style="4" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="5.875" style="1" customWidth="1"/>
+    <col min="2" max="7" width="5.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="5.875" style="1" customWidth="1"/>
+    <col min="10" max="16" width="5.875" style="3" customWidth="1"/>
+    <col min="17" max="26" width="5.875" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -676,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -723,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -770,7 +790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
@@ -817,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -864,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -911,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -958,7 +978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -991,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1008,7 +1028,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1149,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="13"/>
     </row>
-    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1192,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I14" s="19" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I15" s="11" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I17" s="11" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I18" s="15" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
@@ -1301,7 +1321,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
@@ -1348,7 +1368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1442,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1489,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1536,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1583,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1630,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1724,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1771,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -1818,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1865,7 +1885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1912,7 +1932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -1959,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
@@ -2006,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2023,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2091,7 +2111,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -2108,7 +2128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2125,7 +2145,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +2196,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2193,7 +2213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -2208,6 +2228,1371 @@
       </c>
       <c r="E48" s="3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O51" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P51" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q51" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="R51" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="S51" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="T51" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U51" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="12">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="12">
+        <v>5</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0</v>
+      </c>
+      <c r="J52" s="12">
+        <v>0</v>
+      </c>
+      <c r="K52" s="12">
+        <v>0</v>
+      </c>
+      <c r="L52" s="12">
+        <v>0</v>
+      </c>
+      <c r="M52" s="12">
+        <v>0</v>
+      </c>
+      <c r="N52" s="12">
+        <v>0</v>
+      </c>
+      <c r="O52" s="12">
+        <v>0</v>
+      </c>
+      <c r="P52" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>0</v>
+      </c>
+      <c r="R52" s="3">
+        <v>0</v>
+      </c>
+      <c r="S52" s="3">
+        <v>0</v>
+      </c>
+      <c r="T52" s="3">
+        <v>0</v>
+      </c>
+      <c r="U52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="12">
+        <v>0</v>
+      </c>
+      <c r="C53" s="12">
+        <v>0</v>
+      </c>
+      <c r="D53" s="12">
+        <v>0</v>
+      </c>
+      <c r="E53" s="12">
+        <v>0</v>
+      </c>
+      <c r="F53" s="12">
+        <v>2</v>
+      </c>
+      <c r="G53" s="12">
+        <v>7</v>
+      </c>
+      <c r="H53" s="12">
+        <v>0</v>
+      </c>
+      <c r="I53" s="12">
+        <v>0</v>
+      </c>
+      <c r="J53" s="12">
+        <v>0</v>
+      </c>
+      <c r="K53" s="12">
+        <v>0</v>
+      </c>
+      <c r="L53" s="12">
+        <v>0</v>
+      </c>
+      <c r="M53" s="12">
+        <v>0</v>
+      </c>
+      <c r="N53" s="12">
+        <v>0</v>
+      </c>
+      <c r="O53" s="12">
+        <v>0</v>
+      </c>
+      <c r="P53" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="12">
+        <v>0</v>
+      </c>
+      <c r="R53" s="12">
+        <v>0</v>
+      </c>
+      <c r="S53" s="12">
+        <v>0</v>
+      </c>
+      <c r="T53" s="12">
+        <v>0</v>
+      </c>
+      <c r="U53" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="12">
+        <v>0</v>
+      </c>
+      <c r="C54" s="12">
+        <v>0</v>
+      </c>
+      <c r="D54" s="12">
+        <v>0</v>
+      </c>
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>6</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <v>0</v>
+      </c>
+      <c r="J54" s="12">
+        <v>0</v>
+      </c>
+      <c r="K54" s="12">
+        <v>0</v>
+      </c>
+      <c r="L54" s="12">
+        <v>0</v>
+      </c>
+      <c r="M54" s="12">
+        <v>0</v>
+      </c>
+      <c r="N54" s="12">
+        <v>0</v>
+      </c>
+      <c r="O54" s="12">
+        <v>0</v>
+      </c>
+      <c r="P54" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="12">
+        <v>0</v>
+      </c>
+      <c r="R54" s="12">
+        <v>0</v>
+      </c>
+      <c r="S54" s="12">
+        <v>0</v>
+      </c>
+      <c r="T54" s="12">
+        <v>0</v>
+      </c>
+      <c r="U54" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="12">
+        <v>0</v>
+      </c>
+      <c r="C55" s="12">
+        <v>0</v>
+      </c>
+      <c r="D55" s="12">
+        <v>0</v>
+      </c>
+      <c r="E55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0</v>
+      </c>
+      <c r="G55" s="12">
+        <v>1</v>
+      </c>
+      <c r="H55" s="12">
+        <v>0</v>
+      </c>
+      <c r="I55" s="12">
+        <v>0</v>
+      </c>
+      <c r="J55" s="12">
+        <v>0</v>
+      </c>
+      <c r="K55" s="12">
+        <v>0</v>
+      </c>
+      <c r="L55" s="12">
+        <v>0</v>
+      </c>
+      <c r="M55" s="12">
+        <v>0</v>
+      </c>
+      <c r="N55" s="12">
+        <v>0</v>
+      </c>
+      <c r="O55" s="12">
+        <v>0</v>
+      </c>
+      <c r="P55" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="12">
+        <v>0</v>
+      </c>
+      <c r="R55" s="12">
+        <v>0</v>
+      </c>
+      <c r="S55" s="12">
+        <v>0</v>
+      </c>
+      <c r="T55" s="12">
+        <v>0</v>
+      </c>
+      <c r="U55" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="12">
+        <v>0</v>
+      </c>
+      <c r="C56" s="12">
+        <v>0</v>
+      </c>
+      <c r="D56" s="12">
+        <v>0</v>
+      </c>
+      <c r="E56" s="12">
+        <v>0</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>0</v>
+      </c>
+      <c r="H56" s="12">
+        <v>0</v>
+      </c>
+      <c r="I56" s="12">
+        <v>2</v>
+      </c>
+      <c r="J56" s="12">
+        <v>0</v>
+      </c>
+      <c r="K56" s="12">
+        <v>0</v>
+      </c>
+      <c r="L56" s="12">
+        <v>3</v>
+      </c>
+      <c r="M56" s="12">
+        <v>0</v>
+      </c>
+      <c r="N56" s="12">
+        <v>0</v>
+      </c>
+      <c r="O56" s="12">
+        <v>0</v>
+      </c>
+      <c r="P56" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="12">
+        <v>0</v>
+      </c>
+      <c r="R56" s="12">
+        <v>0</v>
+      </c>
+      <c r="S56" s="12">
+        <v>0</v>
+      </c>
+      <c r="T56" s="12">
+        <v>0</v>
+      </c>
+      <c r="U56" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="12">
+        <v>0</v>
+      </c>
+      <c r="C57" s="12">
+        <v>0</v>
+      </c>
+      <c r="D57" s="12">
+        <v>0</v>
+      </c>
+      <c r="E57" s="12">
+        <v>0</v>
+      </c>
+      <c r="F57" s="12">
+        <v>0</v>
+      </c>
+      <c r="G57" s="12">
+        <v>0</v>
+      </c>
+      <c r="H57" s="12">
+        <v>3</v>
+      </c>
+      <c r="I57" s="12">
+        <v>2</v>
+      </c>
+      <c r="J57" s="12">
+        <v>2</v>
+      </c>
+      <c r="K57" s="12">
+        <v>0</v>
+      </c>
+      <c r="L57" s="12">
+        <v>0</v>
+      </c>
+      <c r="M57" s="12">
+        <v>5</v>
+      </c>
+      <c r="N57" s="12">
+        <v>0</v>
+      </c>
+      <c r="O57" s="12">
+        <v>0</v>
+      </c>
+      <c r="P57" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="12">
+        <v>0</v>
+      </c>
+      <c r="R57" s="12">
+        <v>0</v>
+      </c>
+      <c r="S57" s="12">
+        <v>0</v>
+      </c>
+      <c r="T57" s="12">
+        <v>0</v>
+      </c>
+      <c r="U57" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="12">
+        <v>0</v>
+      </c>
+      <c r="C58" s="12">
+        <v>0</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0</v>
+      </c>
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="12">
+        <v>0</v>
+      </c>
+      <c r="G58" s="12">
+        <v>0</v>
+      </c>
+      <c r="H58" s="12">
+        <v>0</v>
+      </c>
+      <c r="I58" s="12">
+        <v>0</v>
+      </c>
+      <c r="J58" s="12">
+        <v>0</v>
+      </c>
+      <c r="K58" s="12">
+        <v>1</v>
+      </c>
+      <c r="L58" s="12">
+        <v>0</v>
+      </c>
+      <c r="M58" s="12">
+        <v>0</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>0</v>
+      </c>
+      <c r="R58" s="12">
+        <v>0</v>
+      </c>
+      <c r="S58" s="12">
+        <v>0</v>
+      </c>
+      <c r="T58" s="12">
+        <v>0</v>
+      </c>
+      <c r="U58" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="12">
+        <v>0</v>
+      </c>
+      <c r="C59" s="12">
+        <v>0</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12">
+        <v>0</v>
+      </c>
+      <c r="F59" s="12">
+        <v>0</v>
+      </c>
+      <c r="G59" s="12">
+        <v>0</v>
+      </c>
+      <c r="H59" s="12">
+        <v>0</v>
+      </c>
+      <c r="I59" s="12">
+        <v>0</v>
+      </c>
+      <c r="J59" s="12">
+        <v>0</v>
+      </c>
+      <c r="K59" s="12">
+        <v>0</v>
+      </c>
+      <c r="L59" s="12">
+        <v>1</v>
+      </c>
+      <c r="M59" s="12">
+        <v>2</v>
+      </c>
+      <c r="N59" s="12">
+        <v>0</v>
+      </c>
+      <c r="O59" s="12">
+        <v>0</v>
+      </c>
+      <c r="P59" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="12">
+        <v>0</v>
+      </c>
+      <c r="R59" s="12">
+        <v>0</v>
+      </c>
+      <c r="S59" s="12">
+        <v>0</v>
+      </c>
+      <c r="T59" s="12">
+        <v>0</v>
+      </c>
+      <c r="U59" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="12">
+        <v>0</v>
+      </c>
+      <c r="C60" s="12">
+        <v>0</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12">
+        <v>0</v>
+      </c>
+      <c r="F60" s="12">
+        <v>0</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0</v>
+      </c>
+      <c r="H60" s="12">
+        <v>0</v>
+      </c>
+      <c r="I60" s="12">
+        <v>0</v>
+      </c>
+      <c r="J60" s="12">
+        <v>0</v>
+      </c>
+      <c r="K60" s="12">
+        <v>0</v>
+      </c>
+      <c r="L60" s="12">
+        <v>0</v>
+      </c>
+      <c r="M60" s="12">
+        <v>0</v>
+      </c>
+      <c r="N60" s="12">
+        <v>3</v>
+      </c>
+      <c r="O60" s="12">
+        <v>0</v>
+      </c>
+      <c r="P60" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="12">
+        <v>0</v>
+      </c>
+      <c r="R60" s="12">
+        <v>0</v>
+      </c>
+      <c r="S60" s="12">
+        <v>0</v>
+      </c>
+      <c r="T60" s="12">
+        <v>0</v>
+      </c>
+      <c r="U60" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="12">
+        <v>0</v>
+      </c>
+      <c r="C61" s="12">
+        <v>0</v>
+      </c>
+      <c r="D61" s="12">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12">
+        <v>0</v>
+      </c>
+      <c r="F61" s="12">
+        <v>0</v>
+      </c>
+      <c r="G61" s="12">
+        <v>0</v>
+      </c>
+      <c r="H61" s="12">
+        <v>0</v>
+      </c>
+      <c r="I61" s="12">
+        <v>0</v>
+      </c>
+      <c r="J61" s="12">
+        <v>0</v>
+      </c>
+      <c r="K61" s="12">
+        <v>0</v>
+      </c>
+      <c r="L61" s="12">
+        <v>0</v>
+      </c>
+      <c r="M61" s="12">
+        <v>0</v>
+      </c>
+      <c r="N61" s="12">
+        <v>0</v>
+      </c>
+      <c r="O61" s="12">
+        <v>0</v>
+      </c>
+      <c r="P61" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="12">
+        <v>3</v>
+      </c>
+      <c r="R61" s="12">
+        <v>0</v>
+      </c>
+      <c r="S61" s="12">
+        <v>0</v>
+      </c>
+      <c r="T61" s="12">
+        <v>8</v>
+      </c>
+      <c r="U61" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="12">
+        <v>0</v>
+      </c>
+      <c r="C62" s="12">
+        <v>0</v>
+      </c>
+      <c r="D62" s="12">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12">
+        <v>0</v>
+      </c>
+      <c r="F62" s="12">
+        <v>0</v>
+      </c>
+      <c r="G62" s="12">
+        <v>0</v>
+      </c>
+      <c r="H62" s="12">
+        <v>0</v>
+      </c>
+      <c r="I62" s="12">
+        <v>0</v>
+      </c>
+      <c r="J62" s="12">
+        <v>0</v>
+      </c>
+      <c r="K62" s="12">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
+        <v>0</v>
+      </c>
+      <c r="M62" s="12">
+        <v>0</v>
+      </c>
+      <c r="N62" s="12">
+        <v>0</v>
+      </c>
+      <c r="O62" s="12">
+        <v>0</v>
+      </c>
+      <c r="P62" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="12">
+        <v>0</v>
+      </c>
+      <c r="R62" s="12">
+        <v>6</v>
+      </c>
+      <c r="S62" s="12">
+        <v>0</v>
+      </c>
+      <c r="T62" s="12">
+        <v>0</v>
+      </c>
+      <c r="U62" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="12">
+        <v>0</v>
+      </c>
+      <c r="C63" s="12">
+        <v>0</v>
+      </c>
+      <c r="D63" s="12">
+        <v>0</v>
+      </c>
+      <c r="E63" s="12">
+        <v>0</v>
+      </c>
+      <c r="F63" s="12">
+        <v>0</v>
+      </c>
+      <c r="G63" s="12">
+        <v>0</v>
+      </c>
+      <c r="H63" s="12">
+        <v>0</v>
+      </c>
+      <c r="I63" s="12">
+        <v>0</v>
+      </c>
+      <c r="J63" s="12">
+        <v>0</v>
+      </c>
+      <c r="K63" s="12">
+        <v>0</v>
+      </c>
+      <c r="L63" s="12">
+        <v>0</v>
+      </c>
+      <c r="M63" s="12">
+        <v>0</v>
+      </c>
+      <c r="N63" s="12">
+        <v>0</v>
+      </c>
+      <c r="O63" s="12">
+        <v>2</v>
+      </c>
+      <c r="P63" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="12">
+        <v>0</v>
+      </c>
+      <c r="R63" s="12">
+        <v>0</v>
+      </c>
+      <c r="S63" s="12">
+        <v>0</v>
+      </c>
+      <c r="T63" s="12">
+        <v>0</v>
+      </c>
+      <c r="U63" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="12">
+        <v>0</v>
+      </c>
+      <c r="C64" s="12">
+        <v>0</v>
+      </c>
+      <c r="D64" s="12">
+        <v>0</v>
+      </c>
+      <c r="E64" s="12">
+        <v>0</v>
+      </c>
+      <c r="F64" s="12">
+        <v>0</v>
+      </c>
+      <c r="G64" s="12">
+        <v>0</v>
+      </c>
+      <c r="H64" s="12">
+        <v>0</v>
+      </c>
+      <c r="I64" s="12">
+        <v>0</v>
+      </c>
+      <c r="J64" s="12">
+        <v>0</v>
+      </c>
+      <c r="K64" s="12">
+        <v>0</v>
+      </c>
+      <c r="L64" s="12">
+        <v>0</v>
+      </c>
+      <c r="M64" s="12">
+        <v>0</v>
+      </c>
+      <c r="N64" s="12">
+        <v>0</v>
+      </c>
+      <c r="O64" s="12">
+        <v>0</v>
+      </c>
+      <c r="P64" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="12">
+        <v>2</v>
+      </c>
+      <c r="R64" s="12">
+        <v>0</v>
+      </c>
+      <c r="S64" s="12">
+        <v>0</v>
+      </c>
+      <c r="T64" s="12">
+        <v>0</v>
+      </c>
+      <c r="U64" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="12">
+        <v>0</v>
+      </c>
+      <c r="C65" s="12">
+        <v>0</v>
+      </c>
+      <c r="D65" s="12">
+        <v>0</v>
+      </c>
+      <c r="E65" s="12">
+        <v>0</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0</v>
+      </c>
+      <c r="G65" s="12">
+        <v>0</v>
+      </c>
+      <c r="H65" s="12">
+        <v>0</v>
+      </c>
+      <c r="I65" s="12">
+        <v>0</v>
+      </c>
+      <c r="J65" s="12">
+        <v>0</v>
+      </c>
+      <c r="K65" s="12">
+        <v>0</v>
+      </c>
+      <c r="L65" s="12">
+        <v>0</v>
+      </c>
+      <c r="M65" s="12">
+        <v>0</v>
+      </c>
+      <c r="N65" s="12">
+        <v>0</v>
+      </c>
+      <c r="O65" s="12">
+        <v>0</v>
+      </c>
+      <c r="P65" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="12">
+        <v>0</v>
+      </c>
+      <c r="R65" s="12">
+        <v>0</v>
+      </c>
+      <c r="S65" s="12">
+        <v>0</v>
+      </c>
+      <c r="T65" s="12">
+        <v>0</v>
+      </c>
+      <c r="U65" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="12">
+        <v>0</v>
+      </c>
+      <c r="C66" s="12">
+        <v>0</v>
+      </c>
+      <c r="D66" s="12">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12">
+        <v>0</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0</v>
+      </c>
+      <c r="G66" s="12">
+        <v>0</v>
+      </c>
+      <c r="H66" s="12">
+        <v>0</v>
+      </c>
+      <c r="I66" s="12">
+        <v>0</v>
+      </c>
+      <c r="J66" s="12">
+        <v>0</v>
+      </c>
+      <c r="K66" s="12">
+        <v>0</v>
+      </c>
+      <c r="L66" s="12">
+        <v>0</v>
+      </c>
+      <c r="M66" s="12">
+        <v>0</v>
+      </c>
+      <c r="N66" s="12">
+        <v>0</v>
+      </c>
+      <c r="O66" s="12">
+        <v>0</v>
+      </c>
+      <c r="P66" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="12">
+        <v>0</v>
+      </c>
+      <c r="R66" s="12">
+        <v>4</v>
+      </c>
+      <c r="S66" s="12">
+        <v>2</v>
+      </c>
+      <c r="T66" s="12">
+        <v>0</v>
+      </c>
+      <c r="U66" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="12">
+        <v>0</v>
+      </c>
+      <c r="C67" s="12">
+        <v>0</v>
+      </c>
+      <c r="D67" s="12">
+        <v>0</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="12">
+        <v>0</v>
+      </c>
+      <c r="H67" s="12">
+        <v>0</v>
+      </c>
+      <c r="I67" s="12">
+        <v>0</v>
+      </c>
+      <c r="J67" s="12">
+        <v>0</v>
+      </c>
+      <c r="K67" s="12">
+        <v>0</v>
+      </c>
+      <c r="L67" s="12">
+        <v>0</v>
+      </c>
+      <c r="M67" s="12">
+        <v>0</v>
+      </c>
+      <c r="N67" s="12">
+        <v>0</v>
+      </c>
+      <c r="O67" s="12">
+        <v>0</v>
+      </c>
+      <c r="P67" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="12">
+        <v>0</v>
+      </c>
+      <c r="R67" s="12">
+        <v>0</v>
+      </c>
+      <c r="S67" s="12">
+        <v>0</v>
+      </c>
+      <c r="T67" s="12">
+        <v>3</v>
+      </c>
+      <c r="U67" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="12">
+        <v>0</v>
+      </c>
+      <c r="C68" s="12">
+        <v>0</v>
+      </c>
+      <c r="D68" s="12">
+        <v>0</v>
+      </c>
+      <c r="E68" s="12">
+        <v>0</v>
+      </c>
+      <c r="F68" s="12">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
+        <v>0</v>
+      </c>
+      <c r="H68" s="12">
+        <v>0</v>
+      </c>
+      <c r="I68" s="12">
+        <v>0</v>
+      </c>
+      <c r="J68" s="12">
+        <v>0</v>
+      </c>
+      <c r="K68" s="12">
+        <v>0</v>
+      </c>
+      <c r="L68" s="12">
+        <v>0</v>
+      </c>
+      <c r="M68" s="12">
+        <v>0</v>
+      </c>
+      <c r="N68" s="12">
+        <v>0</v>
+      </c>
+      <c r="O68" s="12">
+        <v>0</v>
+      </c>
+      <c r="P68" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="12">
+        <v>0</v>
+      </c>
+      <c r="R68" s="12">
+        <v>0</v>
+      </c>
+      <c r="S68" s="12">
+        <v>0</v>
+      </c>
+      <c r="T68" s="12">
+        <v>0</v>
+      </c>
+      <c r="U68" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="12">
+        <v>0</v>
+      </c>
+      <c r="C69" s="12">
+        <v>0</v>
+      </c>
+      <c r="D69" s="12">
+        <v>0</v>
+      </c>
+      <c r="E69" s="12">
+        <v>0</v>
+      </c>
+      <c r="F69" s="12">
+        <v>0</v>
+      </c>
+      <c r="G69" s="12">
+        <v>0</v>
+      </c>
+      <c r="H69" s="12">
+        <v>0</v>
+      </c>
+      <c r="I69" s="12">
+        <v>0</v>
+      </c>
+      <c r="J69" s="12">
+        <v>0</v>
+      </c>
+      <c r="K69" s="12">
+        <v>0</v>
+      </c>
+      <c r="L69" s="12">
+        <v>0</v>
+      </c>
+      <c r="M69" s="12">
+        <v>0</v>
+      </c>
+      <c r="N69" s="12">
+        <v>0</v>
+      </c>
+      <c r="O69" s="12">
+        <v>0</v>
+      </c>
+      <c r="P69" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="12">
+        <v>0</v>
+      </c>
+      <c r="R69" s="12">
+        <v>0</v>
+      </c>
+      <c r="S69" s="12">
+        <v>0</v>
+      </c>
+      <c r="T69" s="12">
+        <v>0</v>
+      </c>
+      <c r="U69" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="12">
+        <v>0</v>
+      </c>
+      <c r="C70" s="12">
+        <v>0</v>
+      </c>
+      <c r="D70" s="12">
+        <v>0</v>
+      </c>
+      <c r="E70" s="12">
+        <v>0</v>
+      </c>
+      <c r="F70" s="12">
+        <v>0</v>
+      </c>
+      <c r="G70" s="12">
+        <v>0</v>
+      </c>
+      <c r="H70" s="12">
+        <v>0</v>
+      </c>
+      <c r="I70" s="12">
+        <v>0</v>
+      </c>
+      <c r="J70" s="12">
+        <v>0</v>
+      </c>
+      <c r="K70" s="12">
+        <v>0</v>
+      </c>
+      <c r="L70" s="12">
+        <v>0</v>
+      </c>
+      <c r="M70" s="12">
+        <v>0</v>
+      </c>
+      <c r="N70" s="12">
+        <v>0</v>
+      </c>
+      <c r="O70" s="12">
+        <v>0</v>
+      </c>
+      <c r="P70" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="12">
+        <v>0</v>
+      </c>
+      <c r="R70" s="12">
+        <v>0</v>
+      </c>
+      <c r="S70" s="12">
+        <v>0</v>
+      </c>
+      <c r="T70" s="12">
+        <v>0</v>
+      </c>
+      <c r="U70" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="12">
+        <v>0</v>
+      </c>
+      <c r="C71" s="12">
+        <v>0</v>
+      </c>
+      <c r="D71" s="12">
+        <v>0</v>
+      </c>
+      <c r="E71" s="12">
+        <v>0</v>
+      </c>
+      <c r="F71" s="12">
+        <v>0</v>
+      </c>
+      <c r="G71" s="12">
+        <v>0</v>
+      </c>
+      <c r="H71" s="12">
+        <v>0</v>
+      </c>
+      <c r="I71" s="12">
+        <v>0</v>
+      </c>
+      <c r="J71" s="12">
+        <v>0</v>
+      </c>
+      <c r="K71" s="12">
+        <v>0</v>
+      </c>
+      <c r="L71" s="12">
+        <v>0</v>
+      </c>
+      <c r="M71" s="12">
+        <v>0</v>
+      </c>
+      <c r="N71" s="12">
+        <v>0</v>
+      </c>
+      <c r="O71" s="12">
+        <v>0</v>
+      </c>
+      <c r="P71" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="12">
+        <v>0</v>
+      </c>
+      <c r="R71" s="12">
+        <v>0</v>
+      </c>
+      <c r="S71" s="12">
+        <v>0</v>
+      </c>
+      <c r="T71" s="12">
+        <v>0</v>
+      </c>
+      <c r="U71" s="12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2219,5 +3604,6 @@
     <sortCondition ref="M10:M18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>